<commit_message>
refactor: more var changes
</commit_message>
<xml_diff>
--- a/Inputs/MasterTable.xlsx
+++ b/Inputs/MasterTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoz\Desktop\WFH\Brown Workfolder\profound-model\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbessey/PycharmProjects/profound-model/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D371FB5-C561-40A6-9787-A6A604A4AC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF909B57-AC23-FF40-9842-AA19424C7E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37860" windowHeight="18180" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialPop" sheetId="12" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="198">
   <si>
     <t>pe</t>
   </si>
@@ -643,6 +643,12 @@
   <si>
     <t>ODD Fx, range assumed</t>
   </si>
+  <si>
+    <t>mortality_nx</t>
+  </si>
+  <si>
+    <t>init_oud_fx</t>
+  </si>
 </sst>
 </file>
 
@@ -1036,13 +1042,13 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>150</v>
       </c>
@@ -1163,7 +1169,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>151</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -1238,13 +1244,13 @@
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1287,7 +1293,7 @@
         <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -1349,7 +1355,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -1372,7 +1378,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1440,12 +1446,12 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>139</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -1481,12 +1487,12 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>139</v>
       </c>
@@ -1497,7 +1503,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1508,7 +1514,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>0.69699999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>0.81899999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1580,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1596,7 +1602,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1662,7 +1668,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>0.48899999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1695,7 +1701,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1706,7 +1712,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1717,7 +1723,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1728,7 +1734,7 @@
         <v>0.75105263157894742</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1739,7 +1745,7 @@
         <v>0.76700000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1750,7 +1756,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1761,7 +1767,7 @@
         <v>0.74399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1794,7 +1800,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>0.56100000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1816,7 +1822,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1827,7 +1833,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -1838,7 +1844,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1849,7 +1855,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1871,7 +1877,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -1893,7 +1899,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>146</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -1915,7 +1921,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -1936,15 +1942,15 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -1984,9 +1990,9 @@
         <v>0.17524139999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B3" s="14">
         <v>3.7000000000000033E-2</v>
@@ -2001,7 +2007,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2015,7 +2021,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -2023,7 +2029,7 @@
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -2031,7 +2037,7 @@
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
@@ -2039,7 +2045,7 @@
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
@@ -2047,7 +2053,7 @@
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
@@ -2055,7 +2061,7 @@
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
     </row>
-    <row r="17" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
@@ -2063,7 +2069,7 @@
       <c r="T17" s="13"/>
       <c r="U17" s="13"/>
     </row>
-    <row r="18" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
@@ -2071,7 +2077,7 @@
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
     </row>
-    <row r="19" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
@@ -2079,7 +2085,7 @@
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
     </row>
-    <row r="21" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
@@ -2087,7 +2093,7 @@
       <c r="T21" s="17"/>
       <c r="U21" s="17"/>
     </row>
-    <row r="22" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
@@ -2095,7 +2101,7 @@
       <c r="T22" s="17"/>
       <c r="U22" s="17"/>
     </row>
-    <row r="23" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -2103,7 +2109,7 @@
       <c r="T23" s="17"/>
       <c r="U23" s="17"/>
     </row>
-    <row r="24" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -2111,23 +2117,23 @@
       <c r="T24" s="17"/>
       <c r="U24" s="17"/>
     </row>
-    <row r="29" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="S29" s="17"/>
       <c r="T29" s="17"/>
     </row>
-    <row r="30" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="12:22" x14ac:dyDescent="0.2">
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
       <c r="S30" s="17"/>
       <c r="T30" s="17"/>
     </row>
-    <row r="32" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="12:22" x14ac:dyDescent="0.2">
       <c r="O32" s="15"/>
       <c r="V32" s="15"/>
     </row>
-    <row r="33" spans="15:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="15:22" x14ac:dyDescent="0.2">
       <c r="O33" s="15"/>
       <c r="V33" s="15"/>
     </row>
@@ -2144,9 +2150,9 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -2172,7 +2178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -2211,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2232,9 +2238,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -2359,7 +2365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -2648,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2016</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -2898,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -3023,7 +3029,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -3148,7 +3154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -3273,7 +3279,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -3398,7 +3404,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -3661,9 +3667,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -3671,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3679,7 +3685,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -3687,7 +3693,7 @@
         <v>2564</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -3695,7 +3701,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -3703,7 +3709,7 @@
         <v>8007</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2019</v>
       </c>
@@ -3724,13 +3730,13 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="19" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="16.83203125" style="19" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B1" s="19" t="s">
         <v>34</v>
       </c>
@@ -3849,7 +3855,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>34</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>35</v>
       </c>
@@ -4093,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>7</v>
       </c>
@@ -4215,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>141</v>
       </c>
@@ -4337,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>37</v>
       </c>
@@ -4459,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
@@ -4581,7 +4587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>9</v>
       </c>
@@ -4703,7 +4709,7 @@
         <v>1.9736842105263157E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -4825,7 +4831,7 @@
         <v>7.3684210526315783E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -4947,7 +4953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>11</v>
       </c>
@@ -5069,7 +5075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>38</v>
       </c>
@@ -5191,7 +5197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
@@ -5313,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>13</v>
       </c>
@@ -5435,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>39</v>
       </c>
@@ -5557,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
@@ -5679,7 +5685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
@@ -5801,7 +5807,7 @@
         <v>6.5637065637065631E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>15</v>
       </c>
@@ -5923,7 +5929,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>24</v>
       </c>
@@ -6045,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
@@ -6167,7 +6173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>40</v>
       </c>
@@ -6289,7 +6295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>41</v>
       </c>
@@ -6411,7 +6417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>26</v>
       </c>
@@ -6533,7 +6539,7 @@
         <v>8.1967213114754103E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>42</v>
       </c>
@@ -6655,7 +6661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>16</v>
       </c>
@@ -6777,7 +6783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>17</v>
       </c>
@@ -6899,7 +6905,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>18</v>
       </c>
@@ -7021,7 +7027,7 @@
         <v>2.8772753963593658E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>27</v>
       </c>
@@ -7143,7 +7149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>19</v>
       </c>
@@ -7265,7 +7271,7 @@
         <v>2.7018486332753989E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>43</v>
       </c>
@@ -7387,7 +7393,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>20</v>
       </c>
@@ -7509,7 +7515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>21</v>
       </c>
@@ -7631,7 +7637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>44</v>
       </c>
@@ -7753,7 +7759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>28</v>
       </c>
@@ -7875,7 +7881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>36</v>
       </c>
@@ -7997,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>31</v>
       </c>
@@ -8119,7 +8125,7 @@
         <v>9.1923834537097834E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>32</v>
       </c>
@@ -8241,7 +8247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>33</v>
       </c>
@@ -8363,7 +8369,7 @@
         <v>2.6595744680851064E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>45</v>
       </c>
@@ -8485,7 +8491,7 @@
         <v>1.3157894736842105E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>22</v>
       </c>
@@ -8618,9 +8624,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -8646,7 +8652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -8672,7 +8678,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -8698,7 +8704,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -8724,7 +8730,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -8750,7 +8756,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -8776,7 +8782,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>133</v>
       </c>
@@ -8802,7 +8808,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>134</v>
       </c>
@@ -8828,7 +8834,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -8854,7 +8860,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -8893,12 +8899,12 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>102</v>
       </c>
@@ -8909,7 +8915,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>80</v>
       </c>
@@ -8932,7 +8938,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>519</v>
       </c>
@@ -8952,7 +8958,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -8980,7 +8986,7 @@
         <v>0.66779999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -9012,7 +9018,7 @@
         <v>0.33220000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -9038,7 +9044,7 @@
         <v>0.87019999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -9070,7 +9076,7 @@
         <v>0.12980000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -9096,7 +9102,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -9128,7 +9134,7 @@
         <v>6.3999999999999946E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -9154,7 +9160,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -9186,7 +9192,7 @@
         <v>0.26200000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -9218,7 +9224,7 @@
         <v>562.55471999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -9250,7 +9256,7 @@
         <v>38.465279999999964</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -9282,7 +9288,7 @@
         <v>220.64724000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -9314,7 +9320,7 @@
         <v>78.332760000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B17">
         <f>B13/(B13+B14)</f>
         <v>0.94099999999999995</v>
@@ -9340,7 +9346,7 @@
         <v>0.93599999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B18">
         <f>B15/(B15+B16)</f>
         <v>0.72699999999999998</v>
@@ -9366,7 +9372,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>91</v>
       </c>
@@ -9380,7 +9386,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -9404,7 +9410,7 @@
         <v>68.003039999999984</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -9436,7 +9442,7 @@
         <v>0.72380353016563426</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>100</v>
       </c>
@@ -9452,7 +9458,7 @@
         <v>5.7068048774948226</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>101</v>
       </c>
@@ -9485,18 +9491,18 @@
   <dimension ref="A1:CC52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="4" max="8" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -9624,7 +9630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -9791,7 +9797,7 @@
       <c r="CB2" s="7"/>
       <c r="CC2" s="7"/>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -9958,7 +9964,7 @@
       <c r="CB3" s="7"/>
       <c r="CC3" s="7"/>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -10125,7 +10131,7 @@
       <c r="CB4" s="7"/>
       <c r="CC4" s="7"/>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -10292,7 +10298,7 @@
       <c r="CB5" s="7"/>
       <c r="CC5" s="7"/>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -10459,7 +10465,7 @@
       <c r="CB6" s="7"/>
       <c r="CC6" s="7"/>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -10626,7 +10632,7 @@
       <c r="CB7" s="7"/>
       <c r="CC7" s="7"/>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -10754,7 +10760,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -10882,7 +10888,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -11010,7 +11016,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -11138,7 +11144,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -11266,7 +11272,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -11394,7 +11400,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -11522,7 +11528,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -11650,7 +11656,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -11778,7 +11784,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -11906,7 +11912,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -12034,7 +12040,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -12162,7 +12168,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -12290,7 +12296,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -12418,7 +12424,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -12546,7 +12552,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -12674,7 +12680,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -12802,7 +12808,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -12930,7 +12936,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -13058,7 +13064,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -13186,7 +13192,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -13314,7 +13320,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -13442,7 +13448,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -13570,7 +13576,7 @@
         <v>3235</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -13698,7 +13704,7 @@
         <v>2970</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -13826,7 +13832,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -13954,7 +13960,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -14082,7 +14088,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -14210,7 +14216,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -14338,7 +14344,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -14466,7 +14472,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -14594,7 +14600,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -14722,7 +14728,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -14850,7 +14856,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -14978,7 +14984,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -15106,7 +15112,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -15234,7 +15240,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -15362,7 +15368,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -15490,7 +15496,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -15618,7 +15624,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -15746,7 +15752,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -15874,7 +15880,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -16002,7 +16008,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D52" s="4"/>
     </row>
   </sheetData>
@@ -16018,9 +16024,9 @@
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -16031,7 +16037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>181</v>
       </c>
@@ -16042,7 +16048,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>181</v>
       </c>
@@ -16053,7 +16059,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>181</v>
       </c>
@@ -16064,7 +16070,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>181</v>
       </c>
@@ -16075,7 +16081,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>176</v>
       </c>
@@ -16087,7 +16093,7 @@
         <v>0.67931034482758623</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>176</v>
       </c>
@@ -16099,7 +16105,7 @@
         <v>0.72377622377622375</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>176</v>
       </c>
@@ -16111,7 +16117,7 @@
         <v>0.83088235294117652</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>176</v>
       </c>
@@ -16123,7 +16129,7 @@
         <v>0.8359375</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>175</v>
       </c>
@@ -16135,7 +16141,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>175</v>
       </c>
@@ -16147,7 +16153,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>175</v>
       </c>
@@ -16159,7 +16165,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>175</v>
       </c>
@@ -16180,16 +16186,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FBC180-692F-4365-89A2-152D7783C468}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -16218,7 +16224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -16239,7 +16245,7 @@
       </c>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -16260,7 +16266,7 @@
       </c>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -16280,7 +16286,7 @@
         <v>8.6259541200034429E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -16300,7 +16306,7 @@
         <v>1.8575312252222864E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -16320,7 +16326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -16340,7 +16346,7 @@
         <v>5.9488195813894986</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -16360,7 +16366,7 @@
         <v>9.6985186018235687</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>156</v>
       </c>
@@ -16380,7 +16386,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -16400,7 +16406,7 @@
         <v>0.17524139999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -16420,7 +16426,7 @@
         <v>4.500000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -16440,7 +16446,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -16460,7 +16466,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -16480,7 +16486,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>DecisionTree!A5</f>
         <v>OD_911_priv</v>
@@ -16502,7 +16508,7 @@
         <v>0.64066852367688021</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>DecisionTree!A6</f>
         <v>OD_911_pub_mul</v>
@@ -16524,7 +16530,7 @@
         <v>1.377</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -16544,7 +16550,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -16564,7 +16570,7 @@
         <v>0.11579589999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -16581,7 +16587,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -16601,7 +16607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16615,9 +16621,9 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -16649,7 +16655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -16681,7 +16687,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -16710,7 +16716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -16739,7 +16745,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -16768,7 +16774,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -16797,7 +16803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -16826,7 +16832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -16855,7 +16861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -16884,7 +16890,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -16913,7 +16919,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -16942,7 +16948,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -16971,7 +16977,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -17000,7 +17006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -17029,7 +17035,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -17058,7 +17064,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -17087,7 +17093,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -17116,7 +17122,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -17145,7 +17151,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -17174,7 +17180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -17203,7 +17209,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -17232,7 +17238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -17261,7 +17267,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -17290,7 +17296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -17319,7 +17325,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -17348,7 +17354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -17377,7 +17383,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -17406,7 +17412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -17435,7 +17441,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -17464,7 +17470,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -17493,7 +17499,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -17522,7 +17528,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -17551,7 +17557,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -17580,7 +17586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -17609,7 +17615,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -17638,7 +17644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -17667,7 +17673,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -17696,7 +17702,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -17725,7 +17731,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -17754,7 +17760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -17783,7 +17789,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -17812,7 +17818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -17841,7 +17847,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -17870,7 +17876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -17899,7 +17905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -17928,7 +17934,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -17957,7 +17963,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -17986,7 +17992,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -18015,7 +18021,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -18057,9 +18063,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -18091,7 +18097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -18123,7 +18129,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -18152,7 +18158,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -18181,7 +18187,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -18210,7 +18216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -18239,7 +18245,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -18268,7 +18274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -18297,7 +18303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -18326,7 +18332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -18355,7 +18361,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -18384,7 +18390,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -18413,7 +18419,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -18442,7 +18448,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -18471,7 +18477,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -18500,7 +18506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -18529,7 +18535,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -18558,7 +18564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -18587,7 +18593,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -18616,7 +18622,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -18645,7 +18651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -18674,7 +18680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -18703,7 +18709,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -18732,7 +18738,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -18761,7 +18767,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -18790,7 +18796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -18819,7 +18825,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -18848,7 +18854,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -18877,7 +18883,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -18906,7 +18912,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -18935,7 +18941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -18964,7 +18970,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -18993,7 +18999,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -19022,7 +19028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -19051,7 +19057,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -19080,7 +19086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -19109,7 +19115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -19138,7 +19144,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -19167,7 +19173,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -19196,7 +19202,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -19225,7 +19231,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -19254,7 +19260,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -19283,7 +19289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -19312,7 +19318,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -19341,7 +19347,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -19370,7 +19376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -19399,7 +19405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -19428,7 +19434,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -19457,7 +19463,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -19495,19 +19501,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE310753-5FDB-4C95-9210-5EA6DD07A095}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -19542,7 +19548,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -19560,7 +19566,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -19578,7 +19584,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -19595,7 +19601,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -19612,7 +19618,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -19635,9 +19641,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -19662,7 +19668,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>187</v>
       </c>
@@ -19686,7 +19692,7 @@
       </c>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>122</v>
       </c>
@@ -19703,7 +19709,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>122</v>
       </c>
@@ -19720,7 +19726,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>122</v>
       </c>
@@ -19738,14 +19744,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E13" s="3"/>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F18" s="3"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F19" s="3"/>
       <c r="H19" s="4"/>
     </row>
@@ -19762,12 +19768,12 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -19793,7 +19799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -19813,7 +19819,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -19834,13 +19840,13 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>82</v>
       </c>
@@ -19872,7 +19878,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>159</v>
       </c>
@@ -19906,7 +19912,7 @@
       </c>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -19940,7 +19946,7 @@
       </c>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -19971,7 +19977,7 @@
       </c>
       <c r="K4" s="12"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -20002,7 +20008,7 @@
       </c>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -20033,7 +20039,7 @@
       </c>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -20064,7 +20070,7 @@
       </c>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -20112,13 +20118,13 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -20147,7 +20153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -20164,7 +20170,7 @@
         <v>8.6259541200034429E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -20181,7 +20187,7 @@
         <v>1.8575312252222864E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -20192,7 +20198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -20212,7 +20218,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -20232,7 +20238,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -20249,7 +20255,7 @@
         <v>9.6985186018235687</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -20266,7 +20272,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -20299,12 +20305,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -20330,7 +20336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -20338,7 +20344,7 @@
         <v>4.1800000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -20346,7 +20352,7 @@
         <v>2.0199999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -20354,7 +20360,7 @@
         <v>8.2400000000000008E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -20362,7 +20368,7 @@
         <v>5.9500000000000004E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -20370,7 +20376,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -20378,7 +20384,7 @@
         <v>2.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
refactor: general code cleanup and change to master table
Rename and whitespace updates. The master table in its previous form was hard-coded to only allow the full population to be run. In progress: the table will now work from percentages instead of concrete numbers.

BREAKING CHANGE:
</commit_message>
<xml_diff>
--- a/Inputs/MasterTable.xlsx
+++ b/Inputs/MasterTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbessey/PycharmProjects/profound-model/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420F4757-8D0A-5247-9135-7E203C4EF4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91995E2B-A199-E84A-A6B0-4D0906377E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37860" windowHeight="18180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37860" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialPop" sheetId="12" r:id="rId1"/>
@@ -497,9 +497,6 @@
     <t>Westerley</t>
   </si>
   <si>
-    <t>pop.size</t>
-  </si>
-  <si>
     <t>prop.12older</t>
   </si>
   <si>
@@ -648,6 +645,9 @@
   </si>
   <si>
     <t>init_inactive</t>
+  </si>
+  <si>
+    <t>ppl_size</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADE474C-D15B-46D6-BDBE-860BFA9FCA0F}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1079,13 +1079,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
       <c r="C2">
-        <v>1059000</v>
+        <v>909141</v>
       </c>
       <c r="D2" t="s">
         <v>50</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
@@ -1349,15 +1349,15 @@
         <v>0.64066852367688021</v>
       </c>
       <c r="I5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
@@ -1372,10 +1372,10 @@
         <v>1.377</v>
       </c>
       <c r="I6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1412,7 +1412,7 @@
         <v>0.11579589999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G8">
         <v>19</v>
@@ -1422,10 +1422,10 @@
         <v>232</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="23">
         <f>1-C2</f>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="14">
         <v>0.1111111</v>
@@ -1992,7 +1992,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="14">
         <v>3.7000000000000033E-2</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4">
         <v>0.8</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="5">
         <v>0.3</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="5">
         <v>0.7</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -9488,10 +9488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB658D2-F688-4298-B00E-9C23AB00DF3A}">
-  <dimension ref="A1:CC52"/>
+  <dimension ref="A1:CC53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16011,6 +16011,12 @@
     <row r="52" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D52" s="4"/>
     </row>
+    <row r="53" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f>SUM(D2:AP49)</f>
+        <v>909141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16039,7 +16045,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" s="24">
         <v>2016</v>
@@ -16050,7 +16056,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="24">
         <v>2017</v>
@@ -16061,7 +16067,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="24">
         <v>2018</v>
@@ -16072,7 +16078,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" s="24">
         <v>2019</v>
@@ -16083,7 +16089,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B6">
         <v>2016</v>
@@ -16095,7 +16101,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>2017</v>
@@ -16107,7 +16113,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8">
         <v>2018</v>
@@ -16119,7 +16125,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9">
         <v>2019</v>
@@ -16131,7 +16137,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10">
         <v>2016</v>
@@ -16143,7 +16149,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11">
         <v>2017</v>
@@ -16155,7 +16161,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12">
         <v>2018</v>
@@ -16167,7 +16173,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13">
         <v>2019</v>
@@ -16247,7 +16253,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -16268,7 +16274,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -16288,7 +16294,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
@@ -16368,7 +16374,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
@@ -16388,7 +16394,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -16408,7 +16414,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -16428,7 +16434,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
@@ -16448,7 +16454,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
@@ -16468,7 +16474,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
@@ -16572,7 +16578,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
@@ -16589,7 +16595,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
@@ -18126,7 +18132,7 @@
         <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -19501,7 +19507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE310753-5FDB-4C95-9210-5EA6DD07A095}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -19620,7 +19626,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
@@ -19643,7 +19649,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -19662,15 +19668,15 @@
         <v>0.86599999999999999</v>
       </c>
       <c r="J7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -19688,7 +19694,7 @@
         <v>0.1</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K8" s="3"/>
     </row>
@@ -19816,7 +19822,7 @@
         <v>0.17030683340777131</v>
       </c>
       <c r="H2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -19869,7 +19875,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>6</v>
@@ -19880,7 +19886,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2">
         <v>13.3</v>
@@ -19905,16 +19911,16 @@
         <v>34.447000000000003</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3">
         <v>70.2</v>
@@ -19939,16 +19945,16 @@
         <v>181.81799999999998</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4">
         <v>128.80000000000001</v>
@@ -19973,13 +19979,13 @@
         <v>333.59199999999998</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5">
         <v>194.7</v>
@@ -20004,13 +20010,13 @@
         <v>504.27299999999997</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6">
         <v>359.9</v>
@@ -20035,13 +20041,13 @@
         <v>932.14099999999985</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7">
         <v>886.7</v>
@@ -20066,13 +20072,13 @@
         <v>2296.5529999999999</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8">
         <v>4386.1000000000004</v>
@@ -20097,7 +20103,7 @@
         <v>11359.999</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K8" s="12"/>
     </row>
@@ -20155,7 +20161,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
         <v>110</v>
@@ -20172,7 +20178,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
         <v>110</v>
@@ -20189,7 +20195,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
         <v>110</v>
@@ -20203,7 +20209,7 @@
         <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5">
         <v>2.9</v>
@@ -20215,7 +20221,7 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -20223,7 +20229,7 @@
         <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="15">
         <v>2.9950980392156863</v>
@@ -20235,7 +20241,7 @@
         <v>5.9488195813894986</v>
       </c>
       <c r="F6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -20243,7 +20249,7 @@
         <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" s="15">
         <v>5.9153225806451619</v>
@@ -20257,10 +20263,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
         <v>155</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
       </c>
       <c r="C8">
         <v>3.5</v>
@@ -20277,7 +20283,7 @@
         <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -20289,7 +20295,7 @@
         <v>1.2</v>
       </c>
       <c r="I9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor(input-table): update input table for probs
WIP changing input table to allow for probability-based demographics.
</commit_message>
<xml_diff>
--- a/Inputs/MasterTable.xlsx
+++ b/Inputs/MasterTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbessey/PycharmProjects/profound-model/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91995E2B-A199-E84A-A6B0-4D0906377E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54462295-8473-B54E-9E92-D7C2B1823847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37860" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37860" windowHeight="18180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialPop" sheetId="12" r:id="rId1"/>
@@ -1038,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADE474C-D15B-46D6-BDBE-860BFA9FCA0F}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -9488,10 +9488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB658D2-F688-4298-B00E-9C23AB00DF3A}">
-  <dimension ref="A1:CC53"/>
+  <dimension ref="A1:CC52"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16011,12 +16011,6 @@
     <row r="52" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <f>SUM(D2:AP49)</f>
-        <v>909141</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: fix fentanyl exposure among prescription opioid users
</commit_message>
<xml_diff>
--- a/Inputs/MasterTable.xlsx
+++ b/Inputs/MasterTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbessey/PycharmProjects/profound-model/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Desktop\profound-model\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420F4757-8D0A-5247-9135-7E203C4EF4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ED0EC1-C6C8-43E7-AA86-2D491657ABB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37860" windowHeight="18180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12264" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialPop" sheetId="12" r:id="rId1"/>
@@ -43,9 +43,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -54,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="202">
   <si>
     <t>pe</t>
   </si>
@@ -649,30 +647,46 @@
   <si>
     <t>init_inactive</t>
   </si>
+  <si>
+    <t>proportion of prescription opioids from sources other than from doctors (eligible for fentanyl exposure)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>out_prebopioid</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>na</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSDUH</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="177" formatCode="0.00000"/>
+    <numFmt numFmtId="178" formatCode="0.0000"/>
+    <numFmt numFmtId="179" formatCode="0.000"/>
+    <numFmt numFmtId="180" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -680,7 +694,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -688,14 +702,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -730,30 +751,30 @@
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1039,16 +1060,16 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -1077,7 +1098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -1106,7 +1127,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -1136,7 +1157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1169,7 +1190,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -1200,7 +1221,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -1232,6 +1253,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1244,13 +1266,13 @@
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -1282,7 +1304,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1293,7 +1315,7 @@
         <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1311,7 +1333,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1329,7 +1351,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>189</v>
       </c>
@@ -1355,7 +1377,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -1378,7 +1400,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1395,7 +1417,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1429,6 +1451,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J8" r:id="rId1" xr:uid="{15D6B813-A970-440E-AF95-498C36C49594}"/>
     <hyperlink ref="J5" r:id="rId2" xr:uid="{7327CC0B-C88B-4874-A1C8-CDE2C37C2633}"/>
@@ -1446,12 +1469,12 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -1462,7 +1485,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -1475,6 +1498,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1487,12 +1511,12 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -1503,7 +1527,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1514,7 +1538,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1525,7 +1549,7 @@
         <v>0.69699999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -1536,7 +1560,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -1547,7 +1571,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1558,7 +1582,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1569,7 +1593,7 @@
         <v>0.81899999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1580,7 +1604,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1591,7 +1615,7 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1602,7 +1626,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1637,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1624,7 +1648,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1635,7 +1659,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -1646,7 +1670,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1657,7 +1681,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1668,7 +1692,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1679,7 +1703,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -1690,7 +1714,7 @@
         <v>0.48899999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1701,7 +1725,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1736,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1723,7 +1747,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1734,7 +1758,7 @@
         <v>0.75105263157894742</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1745,7 +1769,7 @@
         <v>0.76700000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1756,7 +1780,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1767,7 +1791,7 @@
         <v>0.74399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1778,7 +1802,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1789,7 +1813,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1800,7 +1824,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1811,7 +1835,7 @@
         <v>0.56100000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1822,7 +1846,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1833,7 +1857,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -1844,7 +1868,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1855,7 +1879,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1866,7 +1890,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1877,7 +1901,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1888,7 +1912,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -1899,7 +1923,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -1910,7 +1934,7 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -1921,7 +1945,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -1933,6 +1957,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1945,12 +1970,12 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -1976,7 +2001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>177</v>
       </c>
@@ -1990,7 +2015,7 @@
         <v>0.17524139999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>195</v>
       </c>
@@ -2007,7 +2032,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2021,7 +2046,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -2029,7 +2054,7 @@
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -2037,7 +2062,7 @@
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
@@ -2045,7 +2070,7 @@
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
@@ -2053,7 +2078,7 @@
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
@@ -2061,7 +2086,7 @@
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
     </row>
-    <row r="17" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
@@ -2069,7 +2094,7 @@
       <c r="T17" s="13"/>
       <c r="U17" s="13"/>
     </row>
-    <row r="18" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
@@ -2077,7 +2102,7 @@
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
     </row>
-    <row r="19" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
@@ -2085,7 +2110,7 @@
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
     </row>
-    <row r="21" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
@@ -2093,7 +2118,7 @@
       <c r="T21" s="17"/>
       <c r="U21" s="17"/>
     </row>
-    <row r="22" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
@@ -2101,7 +2126,7 @@
       <c r="T22" s="17"/>
       <c r="U22" s="17"/>
     </row>
-    <row r="23" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -2109,7 +2134,7 @@
       <c r="T23" s="17"/>
       <c r="U23" s="17"/>
     </row>
-    <row r="24" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -2117,27 +2142,28 @@
       <c r="T24" s="17"/>
       <c r="U24" s="17"/>
     </row>
-    <row r="29" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="S29" s="17"/>
       <c r="T29" s="17"/>
     </row>
-    <row r="30" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
       <c r="S30" s="17"/>
       <c r="T30" s="17"/>
     </row>
-    <row r="32" spans="12:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="12:22" x14ac:dyDescent="0.25">
       <c r="O32" s="15"/>
       <c r="V32" s="15"/>
     </row>
-    <row r="33" spans="15:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="15:22" x14ac:dyDescent="0.25">
       <c r="O33" s="15"/>
       <c r="V33" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2150,9 +2176,9 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -2178,7 +2204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -2189,7 +2215,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -2203,7 +2229,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -2217,7 +2243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2226,6 +2252,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2238,9 +2265,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -2365,7 +2392,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -2529,7 +2556,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -2654,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2016</v>
       </c>
@@ -2779,7 +2806,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -2904,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -3029,7 +3056,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -3154,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -3279,7 +3306,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -3404,7 +3431,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -3529,7 +3556,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -3655,6 +3682,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3667,9 +3695,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -3677,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3685,7 +3713,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -3693,7 +3721,7 @@
         <v>2564</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -3701,7 +3729,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -3709,7 +3737,7 @@
         <v>8007</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2019</v>
       </c>
@@ -3718,6 +3746,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3730,13 +3759,13 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="19" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="19"/>
+    <col min="1" max="1" width="16.77734375" style="19" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
         <v>34</v>
       </c>
@@ -3855,7 +3884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>34</v>
       </c>
@@ -3977,7 +4006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>35</v>
       </c>
@@ -4099,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>7</v>
       </c>
@@ -4221,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>140</v>
       </c>
@@ -4343,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>37</v>
       </c>
@@ -4465,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
@@ -4587,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>9</v>
       </c>
@@ -4709,7 +4738,7 @@
         <v>1.9736842105263157E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -4831,7 +4860,7 @@
         <v>7.3684210526315783E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -4953,7 +4982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>11</v>
       </c>
@@ -5075,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>38</v>
       </c>
@@ -5197,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
@@ -5319,7 +5348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>13</v>
       </c>
@@ -5441,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>39</v>
       </c>
@@ -5563,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
@@ -5685,7 +5714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
@@ -5807,7 +5836,7 @@
         <v>6.5637065637065631E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>15</v>
       </c>
@@ -5929,7 +5958,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>24</v>
       </c>
@@ -6051,7 +6080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
@@ -6173,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>40</v>
       </c>
@@ -6295,7 +6324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>41</v>
       </c>
@@ -6417,7 +6446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>26</v>
       </c>
@@ -6539,7 +6568,7 @@
         <v>8.1967213114754103E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>42</v>
       </c>
@@ -6661,7 +6690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>16</v>
       </c>
@@ -6783,7 +6812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>17</v>
       </c>
@@ -6905,7 +6934,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>18</v>
       </c>
@@ -7027,7 +7056,7 @@
         <v>2.8772753963593658E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>27</v>
       </c>
@@ -7149,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>19</v>
       </c>
@@ -7271,7 +7300,7 @@
         <v>2.7018486332753989E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>43</v>
       </c>
@@ -7393,7 +7422,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>20</v>
       </c>
@@ -7515,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>21</v>
       </c>
@@ -7637,7 +7666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>44</v>
       </c>
@@ -7759,7 +7788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>28</v>
       </c>
@@ -7881,7 +7910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>36</v>
       </c>
@@ -8003,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>31</v>
       </c>
@@ -8125,7 +8154,7 @@
         <v>9.1923834537097834E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>32</v>
       </c>
@@ -8247,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>33</v>
       </c>
@@ -8369,7 +8398,7 @@
         <v>2.6595744680851064E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>45</v>
       </c>
@@ -8491,7 +8520,7 @@
         <v>1.3157894736842105E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>22</v>
       </c>
@@ -8614,6 +8643,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8624,9 +8654,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -8652,7 +8682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -8678,7 +8708,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -8704,7 +8734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -8730,7 +8760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -8756,7 +8786,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -8782,7 +8812,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -8808,7 +8838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -8834,7 +8864,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -8860,7 +8890,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -8887,6 +8917,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8899,12 +8930,12 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>102</v>
       </c>
@@ -8915,7 +8946,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>80</v>
       </c>
@@ -8938,7 +8969,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>519</v>
       </c>
@@ -8958,7 +8989,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -8986,7 +9017,7 @@
         <v>0.66779999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -9018,7 +9049,7 @@
         <v>0.33220000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -9044,7 +9075,7 @@
         <v>0.87019999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -9076,7 +9107,7 @@
         <v>0.12980000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -9102,7 +9133,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -9134,7 +9165,7 @@
         <v>6.3999999999999946E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -9160,7 +9191,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -9192,7 +9223,7 @@
         <v>0.26200000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -9224,7 +9255,7 @@
         <v>562.55471999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -9256,7 +9287,7 @@
         <v>38.465279999999964</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -9288,7 +9319,7 @@
         <v>220.64724000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -9320,7 +9351,7 @@
         <v>78.332760000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B13/(B13+B14)</f>
         <v>0.94099999999999995</v>
@@ -9346,7 +9377,7 @@
         <v>0.93599999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>B15/(B15+B16)</f>
         <v>0.72699999999999998</v>
@@ -9372,7 +9403,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>91</v>
       </c>
@@ -9386,7 +9417,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -9410,7 +9441,7 @@
         <v>68.003039999999984</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -9442,7 +9473,7 @@
         <v>0.72380353016563426</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>100</v>
       </c>
@@ -9458,7 +9489,7 @@
         <v>5.7068048774948226</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>101</v>
       </c>
@@ -9479,6 +9510,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{4D626F25-AE3D-43BD-BCDE-4A5EC98FAE02}"/>
   </hyperlinks>
@@ -9494,15 +9526,15 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="8" width="11.1640625" customWidth="1"/>
+    <col min="4" max="8" width="11.109375" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -9630,7 +9662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -9797,7 +9829,7 @@
       <c r="CB2" s="7"/>
       <c r="CC2" s="7"/>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -9964,7 +9996,7 @@
       <c r="CB3" s="7"/>
       <c r="CC3" s="7"/>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -10131,7 +10163,7 @@
       <c r="CB4" s="7"/>
       <c r="CC4" s="7"/>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -10298,7 +10330,7 @@
       <c r="CB5" s="7"/>
       <c r="CC5" s="7"/>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -10465,7 +10497,7 @@
       <c r="CB6" s="7"/>
       <c r="CC6" s="7"/>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -10632,7 +10664,7 @@
       <c r="CB7" s="7"/>
       <c r="CC7" s="7"/>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -10760,7 +10792,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -10888,7 +10920,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -11016,7 +11048,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -11144,7 +11176,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -11272,7 +11304,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -11400,7 +11432,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -11528,7 +11560,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -11656,7 +11688,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -11784,7 +11816,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -11912,7 +11944,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -12040,7 +12072,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -12168,7 +12200,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -12296,7 +12328,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -12424,7 +12456,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -12552,7 +12584,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -12680,7 +12712,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -12808,7 +12840,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -12936,7 +12968,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -13064,7 +13096,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -13192,7 +13224,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -13320,7 +13352,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -13448,7 +13480,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -13576,7 +13608,7 @@
         <v>3235</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -13704,7 +13736,7 @@
         <v>2970</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -13832,7 +13864,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -13960,7 +13992,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -14088,7 +14120,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -14216,7 +14248,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -14344,7 +14376,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -14472,7 +14504,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -14600,7 +14632,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -14728,7 +14760,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -14856,7 +14888,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -14984,7 +15016,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -15112,7 +15144,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -15240,7 +15272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -15368,7 +15400,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -15496,7 +15528,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -15624,7 +15656,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -15752,7 +15784,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -15880,7 +15912,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -16008,10 +16040,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16024,9 +16057,9 @@
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -16037,7 +16070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>180</v>
       </c>
@@ -16048,7 +16081,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>180</v>
       </c>
@@ -16059,7 +16092,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>180</v>
       </c>
@@ -16070,7 +16103,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>180</v>
       </c>
@@ -16081,7 +16114,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>175</v>
       </c>
@@ -16093,7 +16126,7 @@
         <v>0.67931034482758623</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>175</v>
       </c>
@@ -16105,7 +16138,7 @@
         <v>0.72377622377622375</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>175</v>
       </c>
@@ -16117,7 +16150,7 @@
         <v>0.83088235294117652</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>175</v>
       </c>
@@ -16129,7 +16162,7 @@
         <v>0.8359375</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>174</v>
       </c>
@@ -16141,7 +16174,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>174</v>
       </c>
@@ -16153,7 +16186,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -16165,7 +16198,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -16178,6 +16211,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16190,12 +16224,12 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -16224,7 +16258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -16245,7 +16279,7 @@
       </c>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -16266,7 +16300,7 @@
       </c>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>152</v>
       </c>
@@ -16286,7 +16320,7 @@
         <v>8.6259541200034429E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -16306,7 +16340,7 @@
         <v>1.8575312252222864E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -16326,7 +16360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -16346,7 +16380,7 @@
         <v>5.9488195813894986</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -16366,7 +16400,7 @@
         <v>9.6985186018235687</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -16386,7 +16420,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -16406,7 +16440,7 @@
         <v>0.17524139999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>178</v>
       </c>
@@ -16426,7 +16460,7 @@
         <v>4.500000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>179</v>
       </c>
@@ -16446,7 +16480,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>183</v>
       </c>
@@ -16466,7 +16500,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -16486,7 +16520,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>DecisionTree!A5</f>
         <v>OD_911_priv</v>
@@ -16508,7 +16542,7 @@
         <v>0.64066852367688021</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>DecisionTree!A6</f>
         <v>OD_911_pub_mul</v>
@@ -16530,7 +16564,7 @@
         <v>1.377</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -16550,7 +16584,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -16570,7 +16604,7 @@
         <v>0.11579589999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>168</v>
       </c>
@@ -16587,7 +16621,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>171</v>
       </c>
@@ -16607,8 +16641,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16618,12 +16653,12 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -16655,7 +16690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -16687,7 +16722,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -16716,7 +16751,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -16745,7 +16780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -16774,7 +16809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -16803,7 +16838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -16832,7 +16867,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -16861,7 +16896,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -16890,7 +16925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -16919,7 +16954,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -16948,7 +16983,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -16977,7 +17012,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -17006,7 +17041,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -17035,7 +17070,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -17064,7 +17099,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -17093,7 +17128,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -17122,7 +17157,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -17151,7 +17186,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -17180,7 +17215,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -17209,7 +17244,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -17238,7 +17273,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -17267,7 +17302,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -17296,7 +17331,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -17325,7 +17360,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -17354,7 +17389,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -17383,7 +17418,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -17412,7 +17447,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -17441,7 +17476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -17470,7 +17505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -17499,7 +17534,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -17528,7 +17563,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -17557,7 +17592,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -17586,7 +17621,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -17615,7 +17650,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -17644,7 +17679,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -17673,7 +17708,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -17702,7 +17737,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -17731,7 +17766,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -17760,7 +17795,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -17789,7 +17824,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -17818,7 +17853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -17847,7 +17882,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -17876,7 +17911,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -17905,7 +17940,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -17934,7 +17969,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -17963,7 +17998,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -17992,7 +18027,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -18021,7 +18056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -18051,6 +18086,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18063,9 +18099,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -18097,7 +18133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -18129,7 +18165,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -18158,7 +18194,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -18187,7 +18223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -18216,7 +18252,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -18245,7 +18281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -18274,7 +18310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -18303,7 +18339,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -18332,7 +18368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -18361,7 +18397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -18390,7 +18426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -18419,7 +18455,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -18448,7 +18484,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -18477,7 +18513,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -18506,7 +18542,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -18535,7 +18571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -18564,7 +18600,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -18593,7 +18629,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -18622,7 +18658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -18651,7 +18687,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -18680,7 +18716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -18709,7 +18745,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -18738,7 +18774,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -18767,7 +18803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -18796,7 +18832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -18825,7 +18861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -18854,7 +18890,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -18883,7 +18919,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -18912,7 +18948,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -18941,7 +18977,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -18970,7 +19006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -18999,7 +19035,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -19028,7 +19064,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -19057,7 +19093,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -19086,7 +19122,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -19115,7 +19151,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -19144,7 +19180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -19173,7 +19209,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -19202,7 +19238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -19231,7 +19267,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -19260,7 +19296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -19289,7 +19325,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -19318,7 +19354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -19347,7 +19383,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -19376,7 +19412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -19405,7 +19441,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -19434,7 +19470,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -19463,7 +19499,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -19493,6 +19529,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19502,18 +19539,18 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -19548,7 +19585,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -19566,7 +19603,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -19584,7 +19621,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -19601,7 +19638,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -19618,7 +19655,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -19641,7 +19678,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>196</v>
       </c>
@@ -19668,7 +19705,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>186</v>
       </c>
@@ -19692,7 +19729,7 @@
       </c>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>121</v>
       </c>
@@ -19709,7 +19746,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>121</v>
       </c>
@@ -19726,7 +19763,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>121</v>
       </c>
@@ -19744,19 +19781,41 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.627</v>
+      </c>
+      <c r="J12" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E13" s="3"/>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" s="3"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" s="3"/>
       <c r="H19" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19765,15 +19824,15 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -19799,7 +19858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -19819,7 +19878,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -19828,6 +19887,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19840,13 +19900,13 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>82</v>
       </c>
@@ -19878,7 +19938,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -19912,7 +19972,7 @@
       </c>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -19946,7 +20006,7 @@
       </c>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -19977,7 +20037,7 @@
       </c>
       <c r="K4" s="12"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -20008,7 +20068,7 @@
       </c>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -20039,7 +20099,7 @@
       </c>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -20070,7 +20130,7 @@
       </c>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -20102,6 +20162,7 @@
       <c r="K8" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{55DA9D74-5A33-4C42-807D-F2F93C00D381}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{9C3EACCD-C7A2-4F18-B733-6791FB183874}"/>
@@ -20118,13 +20179,13 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -20153,7 +20214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -20170,7 +20231,7 @@
         <v>8.6259541200034429E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -20187,7 +20248,7 @@
         <v>1.8575312252222864E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -20198,7 +20259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -20218,7 +20279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -20238,7 +20299,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -20255,7 +20316,7 @@
         <v>9.6985186018235687</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -20272,7 +20333,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -20293,6 +20354,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20305,12 +20367,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
@@ -20336,7 +20398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -20344,7 +20406,7 @@
         <v>4.1800000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -20352,7 +20414,7 @@
         <v>2.0199999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -20360,7 +20422,7 @@
         <v>8.2400000000000008E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -20368,7 +20430,7 @@
         <v>5.9500000000000004E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -20376,7 +20438,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -20384,7 +20446,7 @@
         <v>2.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -20393,6 +20455,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix fentanyl exposure among relapsed
</commit_message>
<xml_diff>
--- a/Inputs/MasterTable.xlsx
+++ b/Inputs/MasterTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Desktop\profound-model\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5D79F3-552D-48A2-9766-A1400217F73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2E1420-5137-477E-BDA2-317F90CE4A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="19200" windowHeight="9600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialPop" sheetId="12" r:id="rId1"/>
@@ -19539,7 +19539,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -19792,7 +19792,7 @@
         <v>200</v>
       </c>
       <c r="D12" s="3">
-        <v>0.627</v>
+        <v>0.19234100000000001</v>
       </c>
       <c r="J12" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
Recalibrated results and code cleaning
</commit_message>
<xml_diff>
--- a/Inputs/MasterTable.xlsx
+++ b/Inputs/MasterTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Desktop\profound-model_0113\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C6B0B3-1C2C-4455-A43A-FF035F0C4F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED939F9B-9152-47E1-A3C7-75652CA5E23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="420" windowWidth="22200" windowHeight="7680" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialPop" sheetId="12" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="193">
   <si>
     <t>pe</t>
   </si>
@@ -230,9 +230,6 @@
     <t>LossExp</t>
   </si>
   <si>
-    <t>Avergae number of months a kit is expired/lost and out of circulation</t>
-  </si>
-  <si>
     <t>OD_wit</t>
   </si>
   <si>
@@ -363,9 +360,6 @@
   </si>
   <si>
     <t>c.nlx.kit</t>
-  </si>
-  <si>
-    <t>c.nlx.dtb</t>
   </si>
   <si>
     <t>c.EMS</t>
@@ -536,10 +530,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>previous estimates: 0.111(0.0685,0.175241)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>mor_nx</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -651,6 +641,30 @@
   </si>
   <si>
     <t>monthly growth rate in fentanyl exposure</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avergae number of months a kit is expired/lost and out of circulation</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bird et al.2015</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> et al, 2016</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>c.nlx.dtb.ssp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>c.nlx.dtb.mailevent</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>c.nlx.dtb.healthcare</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1051,7 +1065,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1062,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>46</v>
@@ -1091,7 +1105,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
@@ -1115,12 +1129,12 @@
         <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -1145,12 +1159,12 @@
         <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -1165,7 +1179,7 @@
         <v>6.7199999999999996E-2</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="7">
         <f>C4</f>
@@ -1176,14 +1190,14 @@
         <v>7.7551020408163258E-3</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -1198,23 +1212,23 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G6" si="0">C5</f>
+        <f>C5</f>
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H6" si="1">(E5-D5)/2/1.96</f>
+        <f>(E5-D5)/2/1.96</f>
         <v>2.5510204081632651E-3</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
@@ -1229,18 +1243,18 @@
         <v>1.9E-2</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="7">
-        <f t="shared" si="0"/>
+        <f>C6</f>
         <v>1.6E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f>(E6-D6)/2/1.96</f>
         <v>1.5306122448979593E-3</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1254,7 +1268,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1264,7 +1278,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1288,12 +1302,12 @@
         <v>6</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2">
         <v>0.12</v>
@@ -1307,7 +1321,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="14">
         <v>0.64500000000000002</v>
@@ -1322,7 +1336,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B4" s="14">
         <v>0.82</v>
@@ -1336,7 +1350,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B5" s="14">
         <v>0.6</v>
@@ -1350,7 +1364,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B6" s="14">
         <v>0.66200000000000003</v>
@@ -1363,15 +1377,15 @@
         <v>0.79900000000000004</v>
       </c>
       <c r="H6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I6" s="22" t="s">
         <v>163</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B7" s="15">
         <v>0.59</v>
@@ -1383,15 +1397,15 @@
         <v>0.7</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="14">
         <v>0.9</v>
@@ -1405,7 +1419,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B9" s="14">
         <v>7.5600000000000001E-2</v>
@@ -1417,7 +1431,7 @@
         <v>0.11579589999999999</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F9">
         <v>19</v>
@@ -1427,10 +1441,10 @@
         <v>232</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1448,7 +1462,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1458,18 +1472,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="23">
         <f>1-C2</f>
@@ -1490,7 +1504,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1500,13 +1514,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1533,7 +1547,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="13">
         <v>0.16700000000000001</v>
@@ -1544,7 +1558,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="13">
         <v>0.29899999999999999</v>
@@ -1643,7 +1657,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14" s="13">
         <v>0.32100000000000001</v>
@@ -1687,7 +1701,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B18" s="13">
         <v>0.51100000000000001</v>
@@ -1841,7 +1855,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B32" s="13">
         <v>0.22600000000000001</v>
@@ -1896,7 +1910,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B37" s="13">
         <v>0.33300000000000002</v>
@@ -1907,7 +1921,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" s="13">
         <v>0.13900000000000001</v>
@@ -1918,7 +1932,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B39" s="13">
         <v>0.19800000000000001</v>
@@ -1949,7 +1963,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1959,7 +1973,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1985,7 +1999,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" s="9">
         <f>9/153</f>
@@ -1998,7 +2012,7 @@
         <v>0.108</v>
       </c>
       <c r="E2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F2">
         <v>9</v>
@@ -2007,12 +2021,12 @@
         <v>153</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B3" s="9">
         <v>8.5599999999999999E-3</v>
@@ -2024,7 +2038,7 @@
         <v>1.32E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F3">
         <v>20</v>
@@ -2032,12 +2046,14 @@
       <c r="G3" s="17">
         <v>2336</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>189</v>
+      </c>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B4">
         <v>0.58799999999999997</v>
@@ -2176,15 +2192,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE6D060-BD9A-4D96-B4CE-F2ECE1E1EF2B}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -2216,12 +2232,12 @@
         <v>15.5</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -2235,7 +2251,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2243,7 +2259,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B5">
         <v>2.69</v>
@@ -2274,7 +2290,7 @@
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
@@ -3023,7 +3039,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3079,7 +3095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6B4D2B-1423-4BB1-B82C-0D272D8DA6C7}">
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -3576,7 +3592,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="20">
         <v>0</v>
@@ -7974,17 +7990,17 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC045363-D7FC-49B9-A9BB-CFCFB09307A2}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -8010,7 +8026,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2">
         <v>1019</v>
@@ -8036,7 +8052,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3">
         <v>1511</v>
@@ -8062,7 +8078,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4">
         <v>1511</v>
@@ -8088,7 +8104,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>631</v>
@@ -8114,9 +8130,9 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="5">
+        <v>101</v>
+      </c>
+      <c r="B6" s="6">
         <v>2000</v>
       </c>
       <c r="C6" t="s">
@@ -8140,10 +8156,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7">
-        <v>61.5</v>
+        <v>55.2</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
@@ -8166,10 +8182,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>190</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
@@ -8192,10 +8208,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>191</v>
       </c>
       <c r="B9">
-        <v>500</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>50</v>
@@ -8218,27 +8234,79 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="5">
+        <v>192</v>
+      </c>
+      <c r="B10">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11">
+        <v>500</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="6">
         <v>1034</v>
       </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
         <v>50</v>
       </c>
     </row>
@@ -8260,10 +8328,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -8271,7 +8339,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" s="24">
         <v>2016</v>
@@ -8282,7 +8350,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" s="24">
         <v>2017</v>
@@ -8293,7 +8361,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="24">
         <v>2018</v>
@@ -8304,7 +8372,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" s="24">
         <v>2019</v>
@@ -8315,7 +8383,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6">
         <v>2016</v>
@@ -8327,7 +8395,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7">
         <v>2017</v>
@@ -8339,7 +8407,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B8">
         <v>2018</v>
@@ -8351,7 +8419,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9">
         <v>2019</v>
@@ -8363,7 +8431,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B10">
         <v>2016</v>
@@ -8375,7 +8443,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B11">
         <v>2017</v>
@@ -8387,7 +8455,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12">
         <v>2018</v>
@@ -8399,7 +8467,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B13">
         <v>2019</v>
@@ -8420,7 +8488,7 @@
   <dimension ref="A1:CC52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8436,10 +8504,10 @@
         <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>34</v>
@@ -8451,7 +8519,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>37</v>
@@ -8564,10 +8632,10 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="11">
         <v>919</v>
@@ -8731,10 +8799,10 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="11">
         <v>462</v>
@@ -8898,10 +8966,10 @@
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="11">
         <v>301</v>
@@ -9065,10 +9133,10 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="11">
         <v>1630</v>
@@ -9232,10 +9300,10 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="11">
         <v>1800</v>
@@ -9399,10 +9467,10 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="11">
         <v>998</v>
@@ -9566,10 +9634,10 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="11">
         <v>6</v>
@@ -9694,10 +9762,10 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="11">
         <v>6</v>
@@ -9822,10 +9890,10 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="11">
         <v>2</v>
@@ -9950,10 +10018,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="11">
         <v>10</v>
@@ -10078,10 +10146,10 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="11">
         <v>6</v>
@@ -10206,10 +10274,10 @@
         <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="11">
         <v>3</v>
@@ -10334,10 +10402,10 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="11">
         <v>28</v>
@@ -10462,10 +10530,10 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="11">
         <v>17</v>
@@ -10590,10 +10658,10 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="11">
         <v>11</v>
@@ -10718,10 +10786,10 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="11">
         <v>33</v>
@@ -10846,10 +10914,10 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="11">
         <v>19</v>
@@ -10974,10 +11042,10 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="11">
         <v>6</v>
@@ -11102,10 +11170,10 @@
         <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="11">
         <v>60</v>
@@ -11230,10 +11298,10 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="11">
         <v>13</v>
@@ -11358,10 +11426,10 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="11">
         <v>16</v>
@@ -11486,10 +11554,10 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="11">
         <v>79</v>
@@ -11614,10 +11682,10 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="11">
         <v>47</v>
@@ -11742,10 +11810,10 @@
         <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="11">
         <v>18</v>
@@ -11870,10 +11938,10 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="11">
         <v>803</v>
@@ -11998,10 +12066,10 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="11">
         <v>367</v>
@@ -12126,10 +12194,10 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="11">
         <v>390</v>
@@ -12254,10 +12322,10 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="11">
         <v>1883</v>
@@ -12382,10 +12450,10 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="11">
         <v>1943</v>
@@ -12510,10 +12578,10 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="11">
         <v>1325</v>
@@ -12638,10 +12706,10 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="11">
         <v>5</v>
@@ -12766,10 +12834,10 @@
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D33" s="11">
         <v>5</v>
@@ -12894,10 +12962,10 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="11">
         <v>3</v>
@@ -13022,10 +13090,10 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="11">
         <v>12</v>
@@ -13150,10 +13218,10 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="11">
         <v>7</v>
@@ -13278,10 +13346,10 @@
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="11">
         <v>3</v>
@@ -13406,10 +13474,10 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="11">
         <v>24</v>
@@ -13534,10 +13602,10 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="11">
         <v>13</v>
@@ -13662,10 +13730,10 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="11">
         <v>14</v>
@@ -13790,10 +13858,10 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="11">
         <v>38</v>
@@ -13918,10 +13986,10 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="11">
         <v>20</v>
@@ -14046,10 +14114,10 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" s="11">
         <v>9</v>
@@ -14174,10 +14242,10 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="11">
         <v>52</v>
@@ -14302,10 +14370,10 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D45" s="11">
         <v>11</v>
@@ -14430,10 +14498,10 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="11">
         <v>21</v>
@@ -14558,10 +14626,10 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D47" s="11">
         <v>92</v>
@@ -14686,10 +14754,10 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" s="11">
         <v>50</v>
@@ -14814,10 +14882,10 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" s="11">
         <v>24</v>
@@ -14951,7 +15019,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14961,7 +15029,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -14987,7 +15055,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="4">
         <f>OpioidPattern!D7</f>
@@ -15005,7 +15073,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B3" s="4">
         <f>OpioidPattern!D8</f>
@@ -15023,7 +15091,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="21">
         <f>OverdoseRisk!C2</f>
@@ -15040,7 +15108,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <f>OverdoseRisk!C3</f>
@@ -15057,7 +15125,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <f>OverdoseRisk!C5</f>
@@ -15074,7 +15142,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="15">
         <f>OverdoseRisk!C6</f>
@@ -15091,7 +15159,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="15">
         <f>OverdoseRisk!C7</f>
@@ -15108,7 +15176,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B9">
         <f>OverdoseRisk!C8</f>
@@ -15125,7 +15193,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B10" s="9">
         <f>Mortality!B2</f>
@@ -15142,7 +15210,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B11" s="9">
         <f>Mortality!B3</f>
@@ -15159,7 +15227,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B12">
         <f>Mortality!B4</f>
@@ -15176,7 +15244,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" s="15">
         <f>DecisionTree!B4</f>
@@ -15211,7 +15279,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15">
         <f>DecisionTree!B8</f>
@@ -15228,7 +15296,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B16" s="14">
         <f>DecisionTree!B9</f>
@@ -15245,7 +15313,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B17">
         <f>NxKit!B3</f>
@@ -15283,10 +15351,10 @@
         <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>0</v>
@@ -15315,10 +15383,10 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="9">
         <v>2.4942686840898669E-2</v>
@@ -15339,7 +15407,7 @@
         <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -15347,10 +15415,10 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="9">
         <v>6.7126436781609192E-2</v>
@@ -15376,10 +15444,10 @@
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="9">
         <v>6.9954776710005648E-2</v>
@@ -15405,10 +15473,10 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="9">
         <v>5.6965357481309889E-2</v>
@@ -15434,10 +15502,10 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="9">
         <v>3.7692145714887347E-2</v>
@@ -15463,10 +15531,10 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="9">
         <v>1.5907447577729574E-2</v>
@@ -15492,10 +15560,10 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="9">
         <v>2.6074182886522218E-2</v>
@@ -15521,10 +15589,10 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="9">
         <v>5.373573794626426E-2</v>
@@ -15550,10 +15618,10 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="9">
         <v>6.8940493468795355E-2</v>
@@ -15579,10 +15647,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="9">
         <v>4.1410184667039732E-2</v>
@@ -15608,10 +15676,10 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="9">
         <v>3.7641154328732745E-2</v>
@@ -15637,10 +15705,10 @@
         <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="9">
         <v>2.5056947608200455E-2</v>
@@ -15666,10 +15734,10 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="9">
         <v>2.436938862761864E-2</v>
@@ -15695,10 +15763,10 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="9">
         <v>6.2884483937115515E-2</v>
@@ -15724,10 +15792,10 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="9">
         <v>5.9245960502692999E-2</v>
@@ -15753,10 +15821,10 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="9">
         <v>4.6042617960426177E-2</v>
@@ -15782,10 +15850,10 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="9">
         <v>2.6683608640406607E-2</v>
@@ -15811,10 +15879,10 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="9">
         <v>2.9069767441860465E-2</v>
@@ -15840,10 +15908,10 @@
         <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="9">
         <v>2.2212908633696564E-2</v>
@@ -15869,10 +15937,10 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="9">
         <v>5.5646481178396073E-2</v>
@@ -15898,10 +15966,10 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="9">
         <v>6.0267857142857144E-2</v>
@@ -15927,10 +15995,10 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="9">
         <v>4.1769041769041768E-2</v>
@@ -15956,10 +16024,10 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="9">
         <v>3.0120481927710843E-2</v>
@@ -15985,10 +16053,10 @@
         <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="9">
         <v>1.7964071856287425E-2</v>
@@ -16014,10 +16082,10 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="9">
         <v>2.7733912356889063E-2</v>
@@ -16043,10 +16111,10 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="9">
         <v>6.7545891997861346E-2</v>
@@ -16072,10 +16140,10 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="9">
         <v>5.9462835727670207E-2</v>
@@ -16101,10 +16169,10 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="9">
         <v>4.374098124098124E-2</v>
@@ -16130,10 +16198,10 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="9">
         <v>3.1348543869411986E-2</v>
@@ -16159,10 +16227,10 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="9">
         <v>1.1685116851168511E-2</v>
@@ -16188,10 +16256,10 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="9">
         <v>3.5166479610924055E-2</v>
@@ -16217,10 +16285,10 @@
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D33" s="9">
         <v>4.6284224250325946E-2</v>
@@ -16246,10 +16314,10 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="9">
         <v>4.4698544698544701E-2</v>
@@ -16275,10 +16343,10 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="9">
         <v>3.0814689742507388E-2</v>
@@ -16304,10 +16372,10 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="9">
         <v>3.125E-2</v>
@@ -16333,10 +16401,10 @@
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="9">
         <v>8.3056478405315621E-3</v>
@@ -16362,10 +16430,10 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="9">
         <v>3.6120840630472856E-2</v>
@@ -16391,10 +16459,10 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="9">
         <v>5.2423777144110548E-2</v>
@@ -16420,10 +16488,10 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="9">
         <v>4.7795479807336047E-2</v>
@@ -16449,10 +16517,10 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="9">
         <v>3.065373787926181E-2</v>
@@ -16478,10 +16546,10 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="9">
         <v>1.3197969543147208E-2</v>
@@ -16507,10 +16575,10 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" s="9">
         <v>2.0876826722338204E-2</v>
@@ -16536,10 +16604,10 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="9">
         <v>3.0328919265271252E-2</v>
@@ -16565,10 +16633,10 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D45" s="9">
         <v>6.0930424042815977E-2</v>
@@ -16594,10 +16662,10 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="9">
         <v>4.7806155861165683E-2</v>
@@ -16623,10 +16691,10 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D47" s="9">
         <v>2.9858849077090119E-2</v>
@@ -16652,10 +16720,10 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" s="9">
         <v>2.3972602739726026E-2</v>
@@ -16681,10 +16749,10 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" s="9">
         <v>1.3927576601671309E-2</v>
@@ -16726,10 +16794,10 @@
         <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>0</v>
@@ -16758,10 +16826,10 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="9">
         <v>3.9431453461714807E-3</v>
@@ -16782,7 +16850,7 @@
         <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -16790,10 +16858,10 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="9">
         <v>5.6091954022988506E-2</v>
@@ -16819,10 +16887,10 @@
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="9">
         <v>4.8473713962690783E-2</v>
@@ -16848,10 +16916,10 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="9">
         <v>2.2428135200589661E-2</v>
@@ -16877,10 +16945,10 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="9">
         <v>1.284480943356496E-2</v>
@@ -16906,10 +16974,10 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="9">
         <v>2.1691973969631237E-3</v>
@@ -16935,10 +17003,10 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="9">
         <v>1.1017260374586854E-3</v>
@@ -16964,10 +17032,10 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="9">
         <v>1.6562384983437616E-2</v>
@@ -16993,10 +17061,10 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="9">
         <v>2.0319303338171262E-2</v>
@@ -17022,10 +17090,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="9">
         <v>1.9026301063234472E-2</v>
@@ -17051,10 +17119,10 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="9">
         <v>3.7641154328732745E-2</v>
@@ -17080,10 +17148,10 @@
         <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="9">
         <v>6.8337129840546698E-3</v>
@@ -17109,10 +17177,10 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="9">
         <v>3.3528918692372171E-3</v>
@@ -17138,10 +17206,10 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="9">
         <v>4.0916530278232409E-2</v>
@@ -17167,10 +17235,10 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="9">
         <v>3.9434523809523808E-2</v>
@@ -17196,10 +17264,10 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="9">
         <v>2.5798525798525797E-2</v>
@@ -17225,10 +17293,10 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="9">
         <v>1.2048192771084338E-2</v>
@@ -17254,10 +17322,10 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="9">
         <v>2.9940119760479044E-3</v>
@@ -17283,10 +17351,10 @@
         <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="9">
         <v>3.8477982043608381E-3</v>
@@ -17312,10 +17380,10 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="9">
         <v>4.5340624287992709E-2</v>
@@ -17341,10 +17409,10 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="9">
         <v>3.7701974865350089E-2</v>
@@ -17370,10 +17438,10 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="9">
         <v>2.5875190258751901E-2</v>
@@ -17399,10 +17467,10 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="9">
         <v>1.5247776365946633E-2</v>
@@ -17428,10 +17496,10 @@
         <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="9">
         <v>5.8139534883720929E-3</v>
@@ -17457,10 +17525,10 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="9">
         <v>3.3557046979865771E-3</v>
@@ -17486,10 +17554,10 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="9">
         <v>3.920869720192479E-2</v>
@@ -17515,10 +17583,10 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="9">
         <v>2.7357901311680199E-2</v>
@@ -17544,10 +17612,10 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="9">
         <v>1.0281385281385282E-2</v>
@@ -17573,10 +17641,10 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="9">
         <v>6.3068076423669081E-3</v>
@@ -17602,10 +17670,10 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="9">
         <v>1.025010250102501E-3</v>
@@ -17631,10 +17699,10 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="9">
         <v>1.4964459408903852E-3</v>
@@ -17660,10 +17728,10 @@
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D33" s="9">
         <v>1.2059973924380704E-2</v>
@@ -17689,10 +17757,10 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="9">
         <v>1.0914760914760915E-2</v>
@@ -17718,10 +17786,10 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="9">
         <v>1.2241452089489235E-2</v>
@@ -17747,10 +17815,10 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="9">
         <v>1.46484375E-2</v>
@@ -17776,10 +17844,10 @@
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="9">
         <v>0</v>
@@ -17805,10 +17873,10 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="9">
         <v>3.8445108927808629E-3</v>
@@ -17834,10 +17902,10 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="9">
         <v>3.1700288184438041E-2</v>
@@ -17863,10 +17931,10 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="9">
         <v>2.2920759659463E-2</v>
@@ -17892,10 +17960,10 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="9">
         <v>1.1400651465798045E-2</v>
@@ -17921,10 +17989,10 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="9">
         <v>5.1369863013698627E-3</v>
@@ -17950,10 +18018,10 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" s="9">
         <v>0</v>
@@ -17979,10 +18047,10 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="9">
         <v>4.5971978984238179E-3</v>
@@ -18008,10 +18076,10 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D45" s="9">
         <v>3.2243913138846239E-2</v>
@@ -18037,10 +18105,10 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="9">
         <v>1.7413856984068173E-2</v>
@@ -18066,10 +18134,10 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D47" s="9">
         <v>1.0009383797309979E-2</v>
@@ -18095,10 +18163,10 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" s="9">
         <v>5.076142131979695E-3</v>
@@ -18124,10 +18192,10 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" s="9">
         <v>0</v>
@@ -18172,13 +18240,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>0</v>
@@ -18202,12 +18270,12 @@
         <v>6</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -18225,7 +18293,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
         <v>52</v>
@@ -18243,7 +18311,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -18260,7 +18328,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
         <v>52</v>
@@ -18277,7 +18345,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
@@ -18300,7 +18368,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -18319,15 +18387,15 @@
         <v>0.86599999999999999</v>
       </c>
       <c r="J7" t="s">
+        <v>149</v>
+      </c>
+      <c r="K7" t="s">
         <v>151</v>
-      </c>
-      <c r="K7" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -18345,13 +18413,13 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>50</v>
@@ -18368,7 +18436,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>50</v>
@@ -18385,7 +18453,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -18403,22 +18471,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D12" s="3">
         <v>0.19234100000000001</v>
       </c>
       <c r="J12" t="s">
+        <v>155</v>
+      </c>
+      <c r="K12" t="s">
         <v>157</v>
-      </c>
-      <c r="K12" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -18444,7 +18512,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -18454,7 +18522,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -18480,7 +18548,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2">
         <f>3587000/(3587000+891000)*0.176+891000/(3587000+891000)*0.079</f>
@@ -18495,12 +18563,12 @@
         <v>0.17030683340777131</v>
       </c>
       <c r="H2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="10">
         <v>0.25244517036746611</v>
@@ -18528,7 +18596,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -18549,18 +18617,18 @@
         <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2">
         <v>13.3</v>
@@ -18581,20 +18649,20 @@
         <v>50</v>
       </c>
       <c r="H2" s="16">
-        <f>B2*2.59</f>
+        <f t="shared" ref="H2:H8" si="0">B2*2.59</f>
         <v>34.447000000000003</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3">
         <v>70.2</v>
@@ -18615,20 +18683,20 @@
         <v>50</v>
       </c>
       <c r="H3" s="16">
-        <f>B3*2.59</f>
+        <f t="shared" si="0"/>
         <v>181.81799999999998</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4">
         <v>128.80000000000001</v>
@@ -18649,17 +18717,17 @@
         <v>50</v>
       </c>
       <c r="H4" s="16">
-        <f t="shared" ref="H4:H8" si="0">B4*2.59</f>
+        <f t="shared" si="0"/>
         <v>333.59199999999998</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B5">
         <v>194.7</v>
@@ -18684,13 +18752,13 @@
         <v>504.27299999999997</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6">
         <v>359.9</v>
@@ -18715,13 +18783,13 @@
         <v>932.14099999999985</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B7">
         <v>886.7</v>
@@ -18746,13 +18814,13 @@
         <v>2296.5529999999999</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B8">
         <v>4386.1000000000004</v>
@@ -18777,7 +18845,7 @@
         <v>11359.999</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K8" s="12"/>
     </row>
@@ -18808,7 +18876,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>57</v>
@@ -18837,10 +18905,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="21">
         <v>2.6026429525052852E-3</v>
@@ -18854,10 +18922,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>1.538E-2</v>
@@ -18871,10 +18939,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -18888,10 +18956,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5">
         <v>3.1</v>
@@ -18903,15 +18971,15 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="26">
         <v>6.0709999999999997</v>
@@ -18923,18 +18991,18 @@
         <v>10.162000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="26">
         <v>4.3</v>
@@ -18946,15 +19014,15 @@
         <v>5.2</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C8">
         <v>3.5</v>
@@ -18966,15 +19034,15 @@
         <v>6.4</v>
       </c>
       <c r="I8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -18986,7 +19054,7 @@
         <v>1.2</v>
       </c>
       <c r="I9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -19005,7 +19073,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:B7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -19015,7 +19083,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -19041,7 +19109,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>4.1800000000000002E-4</v>
@@ -19049,18 +19117,18 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>3.7399999999999998E-3</v>
       </c>
       <c r="H3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>8.2400000000000008E-3</v>
@@ -19068,18 +19136,18 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B5">
         <v>5.9500000000000004E-3</v>
       </c>
       <c r="H5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6">
         <v>1.4800000000000001E-2</v>
@@ -19087,18 +19155,18 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B7">
         <v>2.5400000000000002E-3</v>
       </c>
       <c r="H7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B8">
         <v>4.5199999999999997E-2</v>
@@ -19106,13 +19174,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B9" s="3">
         <v>5.94E-3</v>
       </c>
       <c r="H9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>